<commit_message>
Release 1.1.1 BETA (Linux Default for internetAccess.py)
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,6 +844,1276 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:04:32</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ABAM</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>RMC</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MRG EP Demo</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Issac</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:07:29</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ABAM2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>RMC</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MRG EP Demo</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Issac</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:17:32</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:17:39</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:17:44</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:17:49</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:17:54</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:17:58</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:07</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:15</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:25</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:36</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:42</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:46</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:51</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:18:58</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:19:09</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:19:39</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:22</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:26</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:28</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:33</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:36</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:38</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:41</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:44</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:47</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:49</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:52</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:55</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:20:58</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-10-08 14:21:01</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Delete</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>